<commit_message>
Término da classe Tabela
</commit_message>
<xml_diff>
--- a/DOW/tabelastest/tables2.xlsx
+++ b/DOW/tabelastest/tables2.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="34">
   <si>
     <t xml:space="preserve">Salário Anual Bruto (Milhares de R$)</t>
   </si>
@@ -93,6 +93,36 @@
   </si>
   <si>
     <t xml:space="preserve">Freq. Acumulada Relativa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Salário Mensal Bruto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Freq. Acumulada de Funcionários</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Freq. Relativa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[1700, 2900[</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[2900, 4100[</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[4100, 5300[</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[5300, 6500[</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[6500, 7700[</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[7700, 8900[</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[8900, 10100[</t>
   </si>
 </sst>
 </file>
@@ -209,7 +239,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -242,6 +272,10 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -250,7 +284,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -345,7 +379,7 @@
       <selection pane="topLeft" activeCell="B11" activeCellId="0" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="33.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="23.15"/>
@@ -548,17 +582,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
+      <selection pane="topLeft" activeCell="E14" activeCellId="0" sqref="E14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.64"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="22.6"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="21.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="32.19"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="17.86"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -571,97 +608,185 @@
       <c r="C1" s="7" t="s">
         <v>23</v>
       </c>
+      <c r="E1" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="8" t="n">
+      <c r="A2" s="9" t="n">
         <v>19</v>
       </c>
-      <c r="B2" s="8" t="n">
+      <c r="B2" s="9" t="n">
         <v>25</v>
       </c>
-      <c r="C2" s="9" t="n">
+      <c r="C2" s="10" t="n">
         <f aca="false">B2/B10</f>
         <v>0.125</v>
       </c>
+      <c r="E2" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="F2" s="11" t="n">
+        <v>18</v>
+      </c>
+      <c r="G2" s="11" t="n">
+        <v>18</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="8" t="n">
+      <c r="A3" s="9" t="n">
         <v>20</v>
       </c>
-      <c r="B3" s="10" t="n">
+      <c r="B3" s="8" t="n">
         <v>27</v>
       </c>
-      <c r="C3" s="11" t="n">
+      <c r="C3" s="12" t="n">
         <v>0.26</v>
       </c>
+      <c r="E3" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="F3" s="11" t="n">
+        <v>39</v>
+      </c>
+      <c r="G3" s="11" t="n">
+        <f aca="false">F3-F2</f>
+        <v>21</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="8" t="n">
+      <c r="A4" s="9" t="n">
         <v>21</v>
       </c>
-      <c r="B4" s="8" t="n">
+      <c r="B4" s="9" t="n">
         <v>26</v>
       </c>
-      <c r="C4" s="9" t="n">
+      <c r="C4" s="10" t="n">
         <f aca="false">(B4/B10)+C3</f>
         <v>0.39</v>
       </c>
+      <c r="E4" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="F4" s="11" t="n">
+        <v>64</v>
+      </c>
+      <c r="G4" s="11" t="n">
+        <f aca="false">F4-F3</f>
+        <v>25</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="8" t="n">
+      <c r="A5" s="9" t="n">
         <v>22</v>
       </c>
-      <c r="B5" s="10" t="n">
+      <c r="B5" s="8" t="n">
         <v>24</v>
       </c>
-      <c r="C5" s="11" t="n">
+      <c r="C5" s="12" t="n">
         <v>0.51</v>
       </c>
+      <c r="E5" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="F5" s="11" t="n">
+        <v>93</v>
+      </c>
+      <c r="G5" s="11" t="n">
+        <f aca="false">F5-F4</f>
+        <v>29</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="8" t="n">
+      <c r="A6" s="9" t="n">
         <v>23</v>
       </c>
-      <c r="B6" s="8" t="n">
+      <c r="B6" s="9" t="n">
         <v>29</v>
       </c>
-      <c r="C6" s="9" t="n">
+      <c r="C6" s="10" t="n">
         <f aca="false">(B6/B10)+C5</f>
         <v>0.655</v>
       </c>
+      <c r="E6" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="F6" s="11" t="n">
+        <v>115</v>
+      </c>
+      <c r="G6" s="11" t="n">
+        <f aca="false">F6-F5</f>
+        <v>22</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="8" t="n">
+      <c r="A7" s="9" t="n">
         <v>24</v>
       </c>
-      <c r="B7" s="10" t="n">
+      <c r="B7" s="8" t="n">
         <v>26</v>
       </c>
-      <c r="C7" s="11" t="n">
+      <c r="C7" s="12" t="n">
         <v>0.785</v>
       </c>
+      <c r="E7" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="F7" s="11" t="n">
+        <v>132</v>
+      </c>
+      <c r="G7" s="11" t="n">
+        <f aca="false">F7-F6</f>
+        <v>17</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="8" t="n">
+      <c r="A8" s="9" t="n">
         <v>25</v>
       </c>
-      <c r="B8" s="8" t="n">
+      <c r="B8" s="9" t="n">
         <v>23</v>
       </c>
-      <c r="C8" s="12" t="n">
+      <c r="C8" s="13" t="n">
         <f aca="false">(B8/B10)+C7</f>
         <v>0.9</v>
       </c>
+      <c r="E8" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="F8" s="11" t="n">
+        <v>140</v>
+      </c>
+      <c r="G8" s="11" t="n">
+        <f aca="false">F8-F7</f>
+        <v>8</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="8" t="n">
+      <c r="A9" s="9" t="n">
         <v>26</v>
       </c>
-      <c r="B9" s="10" t="n">
+      <c r="B9" s="8" t="n">
         <v>20</v>
       </c>
-      <c r="C9" s="12" t="n">
+      <c r="C9" s="13" t="n">
         <v>1</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="F9" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="G9" s="8" t="n">
+        <f aca="false">SUM(G2:G8)</f>
+        <v>140</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>